<commit_message>
Added Bastien to category
</commit_message>
<xml_diff>
--- a/website_content_creation/authors/Bastien_Humbert/Author_form.xlsx
+++ b/website_content_creation/authors/Bastien_Humbert/Author_form.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://041gc-my.sharepoint.com/personal/emily_smenderovac_nrcan-rncan_gc_ca/Documents/Documents/WET lab/GLFC-WET.github.io/website_content_creation/authors/Bastien_Humbert/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="23" documentId="8_{4832B352-E1DF-4FFC-9B59-169AA3789519}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DE4019DF-06F9-4D45-A885-2556A73B1338}"/>
+  <xr:revisionPtr revIDLastSave="24" documentId="8_{4832B352-E1DF-4FFC-9B59-169AA3789519}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{057EF722-9B99-4630-B99A-245347F23989}"/>
   <bookViews>
-    <workbookView xWindow="14565" yWindow="-16320" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1788" yWindow="1344" windowWidth="17280" windowHeight="9204" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
     <t>Website Profile Form</t>
   </si>
@@ -139,6 +139,9 @@
   </si>
   <si>
     <t>Summer Intern</t>
+  </si>
+  <si>
+    <t>Visiting and Co-supervised Students</t>
   </si>
 </sst>
 </file>
@@ -155,49 +158,58 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
       <sz val="11"/>
       <color theme="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF1155CC"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0563C1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -555,7 +567,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -590,15 +602,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
@@ -613,6 +616,16 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -831,8 +844,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C1003"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -865,7 +878,7 @@
       <c r="A4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="42" t="s">
+      <c r="B4" s="37" t="s">
         <v>37</v>
       </c>
       <c r="C4" t="s">
@@ -894,7 +907,7 @@
       <c r="A8" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="35" t="s">
+      <c r="B8" s="30" t="s">
         <v>28</v>
       </c>
     </row>
@@ -938,6 +951,9 @@
       <c r="A14" s="17" t="s">
         <v>18</v>
       </c>
+      <c r="B14" s="43" t="s">
+        <v>38</v>
+      </c>
       <c r="C14" t="s">
         <v>22</v>
       </c>
@@ -948,11 +964,11 @@
       </c>
     </row>
     <row r="16" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="30" t="s">
+      <c r="A16" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="B16" s="31"/>
-      <c r="C16" s="32"/>
+      <c r="B16" s="39"/>
+      <c r="C16" s="40"/>
     </row>
     <row r="17" spans="1:3" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="24" t="s">
@@ -969,7 +985,7 @@
       <c r="A18" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="B18" s="36" t="s">
+      <c r="B18" s="31" t="s">
         <v>30</v>
       </c>
       <c r="C18" s="13">
@@ -977,10 +993,10 @@
       </c>
     </row>
     <row r="19" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="37" t="s">
+      <c r="A19" s="32" t="s">
         <v>32</v>
       </c>
-      <c r="B19" s="36" t="s">
+      <c r="B19" s="31" t="s">
         <v>31</v>
       </c>
       <c r="C19" s="14">
@@ -988,13 +1004,13 @@
       </c>
     </row>
     <row r="20" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="38" t="s">
+      <c r="A20" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="B20" s="40" t="s">
+      <c r="B20" s="35" t="s">
         <v>34</v>
       </c>
-      <c r="C20" s="39" t="s">
+      <c r="C20" s="34" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1010,10 +1026,10 @@
     </row>
     <row r="23" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="24" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="33" t="s">
+      <c r="A24" s="41" t="s">
         <v>20</v>
       </c>
-      <c r="B24" s="34"/>
+      <c r="B24" s="42"/>
     </row>
     <row r="25" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="9" t="s">
@@ -1024,7 +1040,7 @@
       </c>
     </row>
     <row r="26" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="41" t="s">
+      <c r="A26" s="36" t="s">
         <v>36</v>
       </c>
       <c r="B26" s="21"/>

</xml_diff>

<commit_message>
Added some temporary interests for Bastien
</commit_message>
<xml_diff>
--- a/website_content_creation/authors/Bastien_Humbert/Author_form.xlsx
+++ b/website_content_creation/authors/Bastien_Humbert/Author_form.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://041gc-my.sharepoint.com/personal/emily_smenderovac_nrcan-rncan_gc_ca/Documents/Documents/WET lab/GLFC-WET.github.io/website_content_creation/authors/Bastien_Humbert/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="24" documentId="8_{4832B352-E1DF-4FFC-9B59-169AA3789519}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{057EF722-9B99-4630-B99A-245347F23989}"/>
+  <xr:revisionPtr revIDLastSave="27" documentId="8_{4832B352-E1DF-4FFC-9B59-169AA3789519}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BCD0DECB-61BB-49E5-896F-CEC5CC3B030F}"/>
   <bookViews>
-    <workbookView xWindow="1788" yWindow="1344" windowWidth="17280" windowHeight="9204" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2235" yWindow="1680" windowWidth="17280" windowHeight="9210" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
   <si>
     <t>Website Profile Form</t>
   </si>
@@ -142,6 +142,15 @@
   </si>
   <si>
     <t>Visiting and Co-supervised Students</t>
+  </si>
+  <si>
+    <t>Outdoors</t>
+  </si>
+  <si>
+    <t>Culinary Arts</t>
+  </si>
+  <si>
+    <t>Biotechnology</t>
   </si>
 </sst>
 </file>
@@ -616,6 +625,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -625,7 +635,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -844,8 +853,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C1003"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -951,7 +960,7 @@
       <c r="A14" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="B14" s="43" t="s">
+      <c r="B14" s="38" t="s">
         <v>38</v>
       </c>
       <c r="C14" t="s">
@@ -964,11 +973,11 @@
       </c>
     </row>
     <row r="16" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="38" t="s">
+      <c r="A16" s="39" t="s">
         <v>11</v>
       </c>
-      <c r="B16" s="39"/>
-      <c r="C16" s="40"/>
+      <c r="B16" s="40"/>
+      <c r="C16" s="41"/>
     </row>
     <row r="17" spans="1:3" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="24" t="s">
@@ -1026,10 +1035,10 @@
     </row>
     <row r="23" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="24" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="41" t="s">
+      <c r="A24" s="42" t="s">
         <v>20</v>
       </c>
-      <c r="B24" s="42"/>
+      <c r="B24" s="43"/>
     </row>
     <row r="25" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="9" t="s">
@@ -1076,13 +1085,19 @@
       </c>
     </row>
     <row r="35" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="12"/>
+      <c r="A35" s="12" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="36" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="27"/>
+      <c r="A36" s="27" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="37" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="28"/>
+      <c r="A37" s="28" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="38" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="22"/>

</xml_diff>